<commit_message>
Date base is taken into account for date formulas
Date base (1900 or 1904) wasn't taken into account in read-cell for
formula date cells.
Now it's fixed. read-cell-value for Cell/CELL_TYPE_NUMERIC doesn't use
date-format? internally, but isn't removed to save backward
compatibility.
However read-cell-value itself doesn't consider date base as it isn't
present in cell value and requires changing method args.
</commit_message>
<xml_diff>
--- a/test/dk/ative/docjure/testdata/datatypes.xlsx
+++ b/test/dk/ative/docjure/testdata/datatypes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14160" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>foo</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -63,30 +63,32 @@
   <si>
     <t>Scientific</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date formulae</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="15">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="165" formatCode="m/d"/>
-    <numFmt numFmtId="166" formatCode="m/d/yy"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="168" formatCode="d\-mmm"/>
-    <numFmt numFmtId="169" formatCode="d\-mmm\-yy"/>
-    <numFmt numFmtId="170" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="171" formatCode="mmm\-yy"/>
-    <numFmt numFmtId="172" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="173" formatCode="mmmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="174" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="175" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy"/>
-    <numFmt numFmtId="177" formatCode="m/d/yy\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="178" formatCode="m/d/yy\ h:mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="14">
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="167" formatCode="d\-mmm"/>
+    <numFmt numFmtId="168" formatCode="d\-mmm\-yy"/>
+    <numFmt numFmtId="169" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="170" formatCode="mmm\-yy"/>
+    <numFmt numFmtId="171" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="172" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="173" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="174" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="175" formatCode="d\-mmm\-yyyy"/>
+    <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="177" formatCode="m/d/yy\ h:mm"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -127,12 +129,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -144,30 +147,35 @@
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -490,25 +498,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="27"/>
+    <col min="1" max="1" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.75" style="27"/>
+    <col min="10" max="10" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -536,8 +545,11 @@
       <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -565,8 +577,12 @@
       <c r="I2" s="28">
         <v>10000000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="34">
+        <f ca="1">NOW()</f>
+        <v>40459.623633449075</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -594,8 +610,12 @@
       <c r="I3" s="28">
         <v>20000000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="21">
+        <f>D3</f>
+        <v>7541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>-1</v>
       </c>
@@ -620,8 +640,12 @@
       <c r="I4" s="28">
         <v>30000000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="18">
+        <f>E4</f>
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>0</v>
       </c>
@@ -643,8 +667,12 @@
       <c r="I5" s="28">
         <v>1E-10</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="24">
+        <f>F5</f>
+        <v>36192.514236111114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1</v>
       </c>
@@ -658,7 +686,7 @@
         <v>9.2592592592592587E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>1000</v>
       </c>
@@ -666,7 +694,7 @@
         <v>38720</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>1000000</v>
       </c>
@@ -674,232 +702,232 @@
         <v>38721</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D9" s="10">
         <v>38722</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D10" s="11">
         <v>38723</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D11" s="12">
         <v>38724</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D12" s="13">
         <v>38725</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D13" s="14">
         <v>38726</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D14" s="15">
         <v>38727</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D15" s="16">
         <v>38728</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D16" s="5">
         <v>38729</v>
       </c>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" s="5">
         <v>38730</v>
       </c>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D18" s="5">
         <v>38731</v>
       </c>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D19" s="5">
         <v>38732</v>
       </c>
     </row>
-    <row r="20" spans="4:4">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20" s="5">
         <v>38733</v>
       </c>
     </row>
-    <row r="21" spans="4:4">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D21" s="5">
         <v>38734</v>
       </c>
     </row>
-    <row r="22" spans="4:4">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D22" s="5">
         <v>38735</v>
       </c>
     </row>
-    <row r="23" spans="4:4">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D23" s="5">
         <v>38736</v>
       </c>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D24" s="5">
         <v>38737</v>
       </c>
     </row>
-    <row r="25" spans="4:4">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D25" s="5">
         <v>38738</v>
       </c>
     </row>
-    <row r="26" spans="4:4">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D26" s="5">
         <v>38739</v>
       </c>
     </row>
-    <row r="27" spans="4:4">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D27" s="5">
         <v>38740</v>
       </c>
     </row>
-    <row r="28" spans="4:4">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D28" s="5">
         <v>38741</v>
       </c>
     </row>
-    <row r="29" spans="4:4">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D29" s="5">
         <v>38742</v>
       </c>
     </row>
-    <row r="30" spans="4:4">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D30" s="5">
         <v>38743</v>
       </c>
     </row>
-    <row r="31" spans="4:4">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D31" s="5">
         <v>38744</v>
       </c>
     </row>
-    <row r="32" spans="4:4">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D32" s="5">
         <v>38745</v>
       </c>
     </row>
-    <row r="33" spans="4:4">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" s="5">
         <v>38746</v>
       </c>
     </row>
-    <row r="34" spans="4:4">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D34" s="5">
         <v>38747</v>
       </c>
     </row>
-    <row r="35" spans="4:4">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D35" s="17">
         <v>38873</v>
       </c>
     </row>
-    <row r="36" spans="4:4">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D36" s="17">
         <v>16958</v>
       </c>
     </row>
-    <row r="37" spans="4:4">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D37" s="29">
         <v>37711</v>
       </c>
     </row>
-    <row r="38" spans="4:4">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D38" s="30">
         <v>37712</v>
       </c>
     </row>
-    <row r="39" spans="4:4">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D39" s="4">
         <v>37713</v>
       </c>
     </row>
-    <row r="40" spans="4:4">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D40" s="31">
         <v>37714</v>
       </c>
     </row>
-    <row r="41" spans="4:4">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D41" s="30">
         <v>37715</v>
       </c>
     </row>
-    <row r="42" spans="4:4">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D42" s="30">
         <v>37716</v>
       </c>
     </row>
-    <row r="43" spans="4:4">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D43" s="21">
         <v>37717</v>
       </c>
     </row>
-    <row r="44" spans="4:4">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D44" s="30">
         <v>37718</v>
       </c>
     </row>
-    <row r="45" spans="4:4">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D45" s="32">
         <v>37719</v>
       </c>
     </row>
-    <row r="46" spans="4:4">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D46" s="32">
         <v>37720</v>
       </c>
     </row>
-    <row r="47" spans="4:4">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D47" s="33">
         <v>37721</v>
       </c>
     </row>
-    <row r="48" spans="4:4">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D48" s="29">
         <v>37722</v>
       </c>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D49" s="29">
         <v>37723</v>
       </c>
     </row>
-    <row r="50" spans="4:4">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D50" s="29">
         <v>37724</v>
       </c>
     </row>
-    <row r="51" spans="4:4">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D51" s="29">
         <v>37725</v>
       </c>
     </row>
-    <row r="52" spans="4:4">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D52" s="29">
         <v>37726</v>
       </c>
     </row>
-    <row r="53" spans="4:4">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D53" s="29">
         <v>37727</v>
       </c>
     </row>
-    <row r="54" spans="4:4">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D54" s="29">
         <v>37728</v>
       </c>

</xml_diff>